<commit_message>
adapted preparation of admin data
</commit_message>
<xml_diff>
--- a/input_data/admin_data/PER/_clean/total-PER.xlsx
+++ b/input_data/admin_data/PER/_clean/total-PER.xlsx
@@ -15,7 +15,250 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>totalpop</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>sh_rent</t>
+  </si>
+  <si>
+    <t>sh_capital</t>
+  </si>
+  <si>
+    <t>sh_labour</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>totalpop</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>sh_rent</t>
+  </si>
+  <si>
+    <t>sh_capital</t>
+  </si>
+  <si>
+    <t>sh_labour</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>totalpop</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>sh_rent</t>
+  </si>
+  <si>
+    <t>sh_capital</t>
+  </si>
+  <si>
+    <t>sh_labour</t>
+  </si>
   <si>
     <t>year</t>
   </si>
@@ -306,34 +549,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
@@ -341,7 +584,7 @@
         <v>2016</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>32052328</v>
@@ -371,7 +614,7 @@
     <row r="3">
       <c r="A3"/>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>32052328</v>
@@ -401,7 +644,7 @@
     <row r="4">
       <c r="A4"/>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>32052328</v>
@@ -431,7 +674,7 @@
     <row r="5">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>32052328</v>
@@ -461,7 +704,7 @@
     <row r="6">
       <c r="A6"/>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <v>32052328</v>
@@ -491,7 +734,7 @@
     <row r="7">
       <c r="A7"/>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="C7">
         <v>32052328</v>
@@ -521,7 +764,7 @@
     <row r="8">
       <c r="A8"/>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>32052328</v>
@@ -551,7 +794,7 @@
     <row r="9">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="C9">
         <v>32052328</v>
@@ -581,7 +824,7 @@
     <row r="10">
       <c r="A10"/>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C10">
         <v>32052328</v>
@@ -611,7 +854,7 @@
     <row r="11">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="C11">
         <v>32052328</v>
@@ -641,7 +884,7 @@
     <row r="12">
       <c r="A12"/>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C12">
         <v>32052328</v>
@@ -671,7 +914,7 @@
     <row r="13">
       <c r="A13"/>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="C13">
         <v>32052328</v>
@@ -701,7 +944,7 @@
     <row r="14">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="C14">
         <v>32052328</v>
@@ -731,7 +974,7 @@
     <row r="15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="C15">
         <v>32052328</v>
@@ -761,7 +1004,7 @@
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="C16">
         <v>32052328</v>
@@ -791,7 +1034,7 @@
     <row r="17">
       <c r="A17"/>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="C17">
         <v>32052328</v>
@@ -821,7 +1064,7 @@
     <row r="18">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="C18">
         <v>32052328</v>
@@ -859,34 +1102,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>129</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>133</v>
       </c>
       <c r="J1" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
@@ -894,7 +1137,7 @@
         <v>2017</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="C2">
         <v>32281556</v>
@@ -924,7 +1167,7 @@
     <row r="3">
       <c r="A3"/>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="C3">
         <v>32281556</v>
@@ -954,7 +1197,7 @@
     <row r="4">
       <c r="A4"/>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="C4">
         <v>32281556</v>
@@ -984,7 +1227,7 @@
     <row r="5">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="C5">
         <v>32281556</v>
@@ -1014,7 +1257,7 @@
     <row r="6">
       <c r="A6"/>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="C6">
         <v>32281556</v>
@@ -1044,7 +1287,7 @@
     <row r="7">
       <c r="A7"/>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <v>32281556</v>
@@ -1074,7 +1317,7 @@
     <row r="8">
       <c r="A8"/>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="C8">
         <v>32281556</v>
@@ -1104,7 +1347,7 @@
     <row r="9">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="C9">
         <v>32281556</v>
@@ -1134,7 +1377,7 @@
     <row r="10">
       <c r="A10"/>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="C10">
         <v>32281556</v>
@@ -1164,7 +1407,7 @@
     <row r="11">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="C11">
         <v>32281556</v>
@@ -1194,7 +1437,7 @@
     <row r="12">
       <c r="A12"/>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="C12">
         <v>32281556</v>
@@ -1224,7 +1467,7 @@
     <row r="13">
       <c r="A13"/>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="C13">
         <v>32281556</v>
@@ -1254,7 +1497,7 @@
     <row r="14">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="C14">
         <v>32281556</v>
@@ -1284,7 +1527,7 @@
     <row r="15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="C15">
         <v>32281556</v>
@@ -1314,7 +1557,7 @@
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="C16">
         <v>32281556</v>
@@ -1344,7 +1587,7 @@
     <row r="17">
       <c r="A17"/>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="C17">
         <v>32281556</v>
@@ -1374,7 +1617,7 @@
     <row r="18">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="C18">
         <v>32281556</v>
@@ -1412,34 +1655,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>155</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>157</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>158</v>
       </c>
       <c r="H1" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="I1" t="s">
-        <v>79</v>
+        <v>160</v>
       </c>
       <c r="J1" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
@@ -1447,7 +1690,7 @@
         <v>2018</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="C2">
         <v>32552004</v>
@@ -1477,7 +1720,7 @@
     <row r="3">
       <c r="A3"/>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="C3">
         <v>32552004</v>
@@ -1507,7 +1750,7 @@
     <row r="4">
       <c r="A4"/>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="C4">
         <v>32552004</v>
@@ -1537,7 +1780,7 @@
     <row r="5">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="C5">
         <v>32552004</v>
@@ -1567,7 +1810,7 @@
     <row r="6">
       <c r="A6"/>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="C6">
         <v>32552004</v>
@@ -1597,7 +1840,7 @@
     <row r="7">
       <c r="A7"/>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="C7">
         <v>32552004</v>
@@ -1627,7 +1870,7 @@
     <row r="8">
       <c r="A8"/>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="C8">
         <v>32552004</v>
@@ -1657,7 +1900,7 @@
     <row r="9">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="C9">
         <v>32552004</v>
@@ -1687,7 +1930,7 @@
     <row r="10">
       <c r="A10"/>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="C10">
         <v>32552004</v>
@@ -1717,7 +1960,7 @@
     <row r="11">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
       <c r="C11">
         <v>32552004</v>
@@ -1747,7 +1990,7 @@
     <row r="12">
       <c r="A12"/>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>147</v>
       </c>
       <c r="C12">
         <v>32552004</v>
@@ -1777,7 +2020,7 @@
     <row r="13">
       <c r="A13"/>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
       <c r="C13">
         <v>32552004</v>
@@ -1807,7 +2050,7 @@
     <row r="14">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="C14">
         <v>32552004</v>
@@ -1837,7 +2080,7 @@
     <row r="15">
       <c r="A15"/>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="C15">
         <v>32552004</v>
@@ -1867,7 +2110,7 @@
     <row r="16">
       <c r="A16"/>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="C16">
         <v>32552004</v>
@@ -1897,7 +2140,7 @@
     <row r="17">
       <c r="A17"/>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>152</v>
       </c>
       <c r="C17">
         <v>32552004</v>
@@ -1927,7 +2170,7 @@
     <row r="18">
       <c r="A18"/>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>153</v>
       </c>
       <c r="C18">
         <v>32552004</v>

</xml_diff>